<commit_message>
Nuevas direcciones para probar el funcionamiento
</commit_message>
<xml_diff>
--- a/direccionesConDelta.xlsx
+++ b/direccionesConDelta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OVS-caminero\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Direccion</t>
   </si>
@@ -168,6 +168,24 @@
   </si>
   <si>
     <t>"-61.03489897810334"</t>
+  </si>
+  <si>
+    <t>Av. 13 740</t>
+  </si>
+  <si>
+    <t>"-34.918351696395646"</t>
+  </si>
+  <si>
+    <t>"-57.958368194341084"</t>
+  </si>
+  <si>
+    <t>Av. 13 716</t>
+  </si>
+  <si>
+    <t>"-34.91798918721827"</t>
+  </si>
+  <si>
+    <t>"-57.9588346727334"</t>
   </si>
 </sst>
 </file>
@@ -486,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,6 +678,26 @@
         <v>47</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>